<commit_message>
uploading docs from google drive
</commit_message>
<xml_diff>
--- a/doc/CS673_SPPP_RiskManagement_team3.xlsx
+++ b/doc/CS673_SPPP_RiskManagement_team3.xlsx
@@ -108,7 +108,7 @@
     <t>Clearly define tasks and assign task leaders.  Communicate progressive updates through Discord, and take advantage of Git features to monitor repository updates.</t>
   </si>
   <si>
-    <t>N/A - development work will start in Iteration 1</t>
+    <t>There was some duplicate work with Docker as well as the creating the Architectural Diagram in Iteration 1. We will strive to communicate better to avoid this occurring in the upcoming iterations.</t>
   </si>
   <si>
     <t xml:space="preserve">Requirements </t>
@@ -126,7 +126,7 @@
     <t>Work to clearly define requirements, and keep requirements updated as project evolves.  Remain flexible to communicate with team to eliminate points of confusion.</t>
   </si>
   <si>
-    <t>N/A - tickets have been created but no descriptions have been added yet</t>
+    <t>This has not been an issue so far</t>
   </si>
   <si>
     <t>Scope creep</t>
@@ -150,9 +150,6 @@
     <t>Open communication within team with ongoing feedback during planning process to ensure amount of work assigned is realistic</t>
   </si>
   <si>
-    <t>Planning has begun with Jira tickets created in our team board</t>
-  </si>
-  <si>
     <t>Technology competence</t>
   </si>
   <si>
@@ -235,6 +232,9 @@
   </si>
   <si>
     <t>Research potential viable options that suits the scope of the project. Get a subscription if truly necessary</t>
+  </si>
+  <si>
+    <t>After initially testing with Heroku, it was decided to move forward with it due to already having it configured, despite the small paywall</t>
   </si>
 </sst>
 </file>
@@ -245,7 +245,7 @@
     <numFmt numFmtId="164" formatCode="mm/dd/yyyy"/>
     <numFmt numFmtId="165" formatCode="m/d"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="6">
     <font>
       <sz val="10.0"/>
       <color rgb="FF000000"/>
@@ -268,11 +268,6 @@
     <font>
       <color rgb="FF000000"/>
       <name val="Arial"/>
-    </font>
-    <font>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11.0"/>
@@ -300,7 +295,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="15">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -313,39 +308,26 @@
     <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0" shrinkToFit="0" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="164" xfId="0" applyAlignment="1" applyFont="1" applyNumberFormat="1">
-      <alignment horizontal="right" readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+      <alignment horizontal="right" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
+      <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="1"/>
+    </xf>
     <xf borderId="0" fillId="2" fontId="4" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="left" shrinkToFit="0" wrapText="1"/>
     </xf>
-    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
-    <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
-      <alignment readingOrder="0"/>
-    </xf>
+    <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyFont="1"/>
+    <xf borderId="0" fillId="0" fontId="5" numFmtId="0" xfId="0" applyFont="1"/>
     <xf borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment horizontal="right" vertical="bottom"/>
     </xf>
@@ -580,7 +562,7 @@
     <col customWidth="1" min="8" max="8" width="14.88"/>
     <col customWidth="1" min="9" max="9" width="14.75"/>
     <col customWidth="1" min="10" max="10" width="18.5"/>
-    <col customWidth="1" min="11" max="11" width="16.38"/>
+    <col customWidth="1" min="11" max="11" width="24.63"/>
     <col customWidth="1" min="12" max="12" width="8.25"/>
   </cols>
   <sheetData>
@@ -609,13 +591,13 @@
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="4" t="s">
+      <c r="D2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="4" t="s">
+      <c r="E2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="F2" s="3" t="s">
         <v>6</v>
       </c>
       <c r="G2" s="3" t="s">
@@ -638,1285 +620,1285 @@
       </c>
     </row>
     <row r="3" ht="50.25" customHeight="1">
-      <c r="A3" s="5" t="s">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="D3" s="8">
+      <c r="D3" s="5">
         <v>2.0</v>
       </c>
-      <c r="E3" s="8">
+      <c r="E3" s="5">
         <v>4.0</v>
       </c>
-      <c r="F3" s="8">
+      <c r="F3" s="5">
         <v>4.0</v>
       </c>
-      <c r="G3" s="9">
+      <c r="G3" s="5">
         <f t="shared" ref="G3:G15" si="1">(6-D3)*(6-E3)*F3</f>
         <v>32</v>
       </c>
-      <c r="H3" s="5" t="s">
+      <c r="H3" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I3" s="10">
+      <c r="I3" s="6">
         <v>45580.0</v>
       </c>
-      <c r="J3" s="7" t="s">
+      <c r="J3" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="K3" s="7" t="s">
+      <c r="K3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="L3" s="7" t="s">
+      <c r="L3" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M3" s="11"/>
-      <c r="N3" s="11"/>
-      <c r="O3" s="11"/>
-      <c r="P3" s="11"/>
-      <c r="Q3" s="11"/>
-      <c r="R3" s="11"/>
-      <c r="S3" s="11"/>
-      <c r="T3" s="11"/>
-      <c r="U3" s="11"/>
-      <c r="V3" s="11"/>
-      <c r="W3" s="11"/>
-      <c r="X3" s="11"/>
-      <c r="Y3" s="11"/>
-      <c r="Z3" s="11"/>
-      <c r="AA3" s="11"/>
+      <c r="M3" s="7"/>
+      <c r="N3" s="7"/>
+      <c r="O3" s="7"/>
+      <c r="P3" s="7"/>
+      <c r="Q3" s="7"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="7"/>
+      <c r="T3" s="7"/>
+      <c r="U3" s="7"/>
+      <c r="V3" s="7"/>
+      <c r="W3" s="7"/>
+      <c r="X3" s="7"/>
+      <c r="Y3" s="7"/>
+      <c r="Z3" s="7"/>
+      <c r="AA3" s="7"/>
     </row>
     <row r="4">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="5">
         <v>5.0</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="5">
         <v>3.0</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="5">
         <v>4.0</v>
       </c>
-      <c r="G4" s="9">
+      <c r="G4" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="H4" s="5" t="s">
+      <c r="H4" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I4" s="10">
+      <c r="I4" s="6">
         <v>45580.0</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="J4" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="K4" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="L4" s="7" t="s">
+      <c r="L4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M4" s="11"/>
-      <c r="N4" s="11"/>
-      <c r="O4" s="11"/>
-      <c r="P4" s="11"/>
-      <c r="Q4" s="11"/>
-      <c r="R4" s="11"/>
-      <c r="S4" s="11"/>
-      <c r="T4" s="11"/>
-      <c r="U4" s="11"/>
-      <c r="V4" s="11"/>
-      <c r="W4" s="11"/>
-      <c r="X4" s="11"/>
-      <c r="Y4" s="11"/>
-      <c r="Z4" s="11"/>
-      <c r="AA4" s="11"/>
+      <c r="M4" s="7"/>
+      <c r="N4" s="7"/>
+      <c r="O4" s="7"/>
+      <c r="P4" s="7"/>
+      <c r="Q4" s="7"/>
+      <c r="R4" s="7"/>
+      <c r="S4" s="7"/>
+      <c r="T4" s="7"/>
+      <c r="U4" s="7"/>
+      <c r="V4" s="7"/>
+      <c r="W4" s="7"/>
+      <c r="X4" s="7"/>
+      <c r="Y4" s="7"/>
+      <c r="Z4" s="7"/>
+      <c r="AA4" s="7"/>
     </row>
     <row r="5">
-      <c r="A5" s="7" t="s">
+      <c r="A5" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B5" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="5" t="s">
+      <c r="C5" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="5">
         <v>3.0</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="5">
         <v>4.0</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="5">
         <v>4.0</v>
       </c>
-      <c r="G5" s="9">
+      <c r="G5" s="5">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="H5" s="5" t="s">
+      <c r="H5" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="I5" s="10">
+      <c r="I5" s="6">
         <v>45580.0</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="J5" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="K5" s="8" t="s">
         <v>29</v>
       </c>
-      <c r="L5" s="7" t="s">
+      <c r="L5" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M5" s="11"/>
-      <c r="N5" s="11"/>
-      <c r="O5" s="11"/>
-      <c r="P5" s="11"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="11"/>
-      <c r="S5" s="11"/>
-      <c r="T5" s="11"/>
-      <c r="U5" s="11"/>
-      <c r="V5" s="11"/>
-      <c r="W5" s="11"/>
-      <c r="X5" s="11"/>
-      <c r="Y5" s="11"/>
-      <c r="Z5" s="11"/>
-      <c r="AA5" s="11"/>
+      <c r="M5" s="7"/>
+      <c r="N5" s="7"/>
+      <c r="O5" s="7"/>
+      <c r="P5" s="7"/>
+      <c r="Q5" s="7"/>
+      <c r="R5" s="7"/>
+      <c r="S5" s="7"/>
+      <c r="T5" s="7"/>
+      <c r="U5" s="7"/>
+      <c r="V5" s="7"/>
+      <c r="W5" s="7"/>
+      <c r="X5" s="7"/>
+      <c r="Y5" s="7"/>
+      <c r="Z5" s="7"/>
+      <c r="AA5" s="7"/>
     </row>
     <row r="6">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B6" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="5">
         <v>3.0</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="5">
         <v>4.0</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="5">
         <v>4.0</v>
       </c>
-      <c r="G6" s="9">
+      <c r="G6" s="5">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="H6" s="5" t="s">
+      <c r="H6" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I6" s="10">
+      <c r="I6" s="6">
         <v>45580.0</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="J6" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="K6" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="L6" s="7" t="s">
+      <c r="L6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M6" s="11"/>
-      <c r="N6" s="11"/>
-      <c r="O6" s="11"/>
-      <c r="P6" s="11"/>
-      <c r="Q6" s="11"/>
-      <c r="R6" s="11"/>
-      <c r="S6" s="11"/>
-      <c r="T6" s="11"/>
-      <c r="U6" s="11"/>
-      <c r="V6" s="11"/>
-      <c r="W6" s="11"/>
-      <c r="X6" s="11"/>
-      <c r="Y6" s="11"/>
-      <c r="Z6" s="11"/>
-      <c r="AA6" s="11"/>
+      <c r="M6" s="7"/>
+      <c r="N6" s="7"/>
+      <c r="O6" s="7"/>
+      <c r="P6" s="7"/>
+      <c r="Q6" s="7"/>
+      <c r="R6" s="7"/>
+      <c r="S6" s="7"/>
+      <c r="T6" s="7"/>
+      <c r="U6" s="7"/>
+      <c r="V6" s="7"/>
+      <c r="W6" s="7"/>
+      <c r="X6" s="7"/>
+      <c r="Y6" s="7"/>
+      <c r="Z6" s="7"/>
+      <c r="AA6" s="7"/>
     </row>
     <row r="7">
-      <c r="A7" s="7" t="s">
+      <c r="A7" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="2" t="s">
         <v>36</v>
       </c>
-      <c r="C7" s="5" t="s">
+      <c r="C7" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="5">
         <v>4.0</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="5">
         <v>4.0</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="5">
         <v>5.0</v>
       </c>
-      <c r="G7" s="9">
+      <c r="G7" s="5">
         <f t="shared" si="1"/>
         <v>20</v>
       </c>
-      <c r="H7" s="5" t="s">
+      <c r="H7" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I7" s="10">
+      <c r="I7" s="6">
         <v>45580.0</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="J7" s="4" t="s">
         <v>38</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L7" s="7" t="s">
+      <c r="K7" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L7" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M7" s="11"/>
-      <c r="N7" s="11"/>
-      <c r="O7" s="11"/>
-      <c r="P7" s="11"/>
-      <c r="Q7" s="11"/>
-      <c r="R7" s="11"/>
-      <c r="S7" s="11"/>
-      <c r="T7" s="11"/>
-      <c r="U7" s="11"/>
-      <c r="V7" s="11"/>
-      <c r="W7" s="11"/>
-      <c r="X7" s="11"/>
-      <c r="Y7" s="11"/>
-      <c r="Z7" s="11"/>
-      <c r="AA7" s="11"/>
+      <c r="M7" s="7"/>
+      <c r="N7" s="7"/>
+      <c r="O7" s="7"/>
+      <c r="P7" s="7"/>
+      <c r="Q7" s="7"/>
+      <c r="R7" s="7"/>
+      <c r="S7" s="7"/>
+      <c r="T7" s="7"/>
+      <c r="U7" s="7"/>
+      <c r="V7" s="7"/>
+      <c r="W7" s="7"/>
+      <c r="X7" s="7"/>
+      <c r="Y7" s="7"/>
+      <c r="Z7" s="7"/>
+      <c r="AA7" s="7"/>
     </row>
     <row r="8">
-      <c r="A8" s="7" t="s">
+      <c r="A8" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="6" t="s">
+      <c r="B8" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="5">
         <v>3.0</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="5">
         <v>4.0</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="5">
         <v>4.0</v>
       </c>
-      <c r="G8" s="9">
+      <c r="G8" s="5">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="10">
+      <c r="I8" s="6">
         <v>45573.0</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="J8" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="K8" s="5" t="s">
+      <c r="K8" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L8" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M8" s="7"/>
+      <c r="N8" s="7"/>
+      <c r="O8" s="7"/>
+      <c r="P8" s="7"/>
+      <c r="Q8" s="7"/>
+      <c r="R8" s="7"/>
+      <c r="S8" s="7"/>
+      <c r="T8" s="7"/>
+      <c r="U8" s="7"/>
+      <c r="V8" s="7"/>
+      <c r="W8" s="7"/>
+      <c r="X8" s="7"/>
+      <c r="Y8" s="7"/>
+      <c r="Z8" s="7"/>
+      <c r="AA8" s="7"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="L8" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M8" s="11"/>
-      <c r="N8" s="11"/>
-      <c r="O8" s="11"/>
-      <c r="P8" s="11"/>
-      <c r="Q8" s="11"/>
-      <c r="R8" s="11"/>
-      <c r="S8" s="11"/>
-      <c r="T8" s="11"/>
-      <c r="U8" s="11"/>
-      <c r="V8" s="11"/>
-      <c r="W8" s="11"/>
-      <c r="X8" s="11"/>
-      <c r="Y8" s="11"/>
-      <c r="Z8" s="11"/>
-      <c r="AA8" s="11"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="7" t="s">
+      <c r="B9" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="C9" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D9" s="9">
+      <c r="D9" s="5">
         <v>3.0</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="5">
         <v>3.0</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="5">
         <v>4.0</v>
       </c>
-      <c r="G9" s="9">
+      <c r="G9" s="5">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="H9" s="5" t="s">
+      <c r="H9" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I9" s="10">
+      <c r="I9" s="6">
         <v>45559.0</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="J9" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>47</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="L9" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M9" s="7"/>
+      <c r="N9" s="7"/>
+      <c r="O9" s="7"/>
+      <c r="P9" s="7"/>
+      <c r="Q9" s="7"/>
+      <c r="R9" s="7"/>
+      <c r="S9" s="7"/>
+      <c r="T9" s="7"/>
+      <c r="U9" s="7"/>
+      <c r="V9" s="7"/>
+      <c r="W9" s="7"/>
+      <c r="X9" s="7"/>
+      <c r="Y9" s="7"/>
+      <c r="Z9" s="7"/>
+      <c r="AA9" s="7"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="L9" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M9" s="11"/>
-      <c r="N9" s="11"/>
-      <c r="O9" s="11"/>
-      <c r="P9" s="11"/>
-      <c r="Q9" s="11"/>
-      <c r="R9" s="11"/>
-      <c r="S9" s="11"/>
-      <c r="T9" s="11"/>
-      <c r="U9" s="11"/>
-      <c r="V9" s="11"/>
-      <c r="W9" s="11"/>
-      <c r="X9" s="11"/>
-      <c r="Y9" s="11"/>
-      <c r="Z9" s="11"/>
-      <c r="AA9" s="11"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D10" s="9">
+      <c r="D10" s="5">
         <v>3.0</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="5">
         <v>3.0</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="5">
         <v>3.0</v>
       </c>
-      <c r="G10" s="9">
+      <c r="G10" s="5">
         <f t="shared" si="1"/>
         <v>27</v>
       </c>
-      <c r="H10" s="5" t="s">
+      <c r="H10" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I10" s="10">
+      <c r="I10" s="6">
         <v>45573.0</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="J10" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="K10" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L10" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M10" s="7"/>
+      <c r="N10" s="7"/>
+      <c r="O10" s="7"/>
+      <c r="P10" s="7"/>
+      <c r="Q10" s="7"/>
+      <c r="R10" s="7"/>
+      <c r="S10" s="7"/>
+      <c r="T10" s="7"/>
+      <c r="U10" s="7"/>
+      <c r="V10" s="7"/>
+      <c r="W10" s="7"/>
+      <c r="X10" s="7"/>
+      <c r="Y10" s="7"/>
+      <c r="Z10" s="7"/>
+      <c r="AA10" s="7"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="L10" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M10" s="11"/>
-      <c r="N10" s="11"/>
-      <c r="O10" s="11"/>
-      <c r="P10" s="11"/>
-      <c r="Q10" s="11"/>
-      <c r="R10" s="11"/>
-      <c r="S10" s="11"/>
-      <c r="T10" s="11"/>
-      <c r="U10" s="11"/>
-      <c r="V10" s="11"/>
-      <c r="W10" s="11"/>
-      <c r="X10" s="11"/>
-      <c r="Y10" s="11"/>
-      <c r="Z10" s="11"/>
-      <c r="AA10" s="11"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="7" t="s">
-        <v>44</v>
-      </c>
-      <c r="B11" s="2" t="s">
+      <c r="C11" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="C11" s="5" t="s">
-        <v>53</v>
-      </c>
-      <c r="D11" s="9">
+      <c r="D11" s="5">
         <v>3.0</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="5">
         <v>2.0</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="5">
         <v>3.0</v>
       </c>
-      <c r="G11" s="9">
+      <c r="G11" s="5">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="H11" s="5" t="s">
+      <c r="H11" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I11" s="10">
+      <c r="I11" s="6">
         <v>45559.0</v>
       </c>
-      <c r="J11" s="5" t="s">
+      <c r="J11" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="K11" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="L11" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M11" s="7"/>
+      <c r="N11" s="7"/>
+      <c r="O11" s="7"/>
+      <c r="P11" s="7"/>
+      <c r="Q11" s="7"/>
+      <c r="R11" s="7"/>
+      <c r="S11" s="7"/>
+      <c r="T11" s="7"/>
+      <c r="U11" s="7"/>
+      <c r="V11" s="7"/>
+      <c r="W11" s="7"/>
+      <c r="X11" s="7"/>
+      <c r="Y11" s="7"/>
+      <c r="Z11" s="7"/>
+      <c r="AA11" s="7"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="K11" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="L11" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M11" s="11"/>
-      <c r="N11" s="11"/>
-      <c r="O11" s="11"/>
-      <c r="P11" s="11"/>
-      <c r="Q11" s="11"/>
-      <c r="R11" s="11"/>
-      <c r="S11" s="11"/>
-      <c r="T11" s="11"/>
-      <c r="U11" s="11"/>
-      <c r="V11" s="11"/>
-      <c r="W11" s="11"/>
-      <c r="X11" s="11"/>
-      <c r="Y11" s="11"/>
-      <c r="Z11" s="11"/>
-      <c r="AA11" s="11"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="7" t="s">
+      <c r="B12" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="C12" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="C12" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="D12" s="9">
+      <c r="D12" s="5">
         <v>3.0</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="5">
         <v>2.0</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="5">
         <v>4.0</v>
       </c>
-      <c r="G12" s="9">
+      <c r="G12" s="5">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="H12" s="5" t="s">
+      <c r="H12" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="I12" s="10">
+      <c r="I12" s="6">
         <v>45580.0</v>
       </c>
-      <c r="J12" s="5" t="s">
+      <c r="J12" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="K12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L12" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M12" s="7"/>
+      <c r="N12" s="7"/>
+      <c r="O12" s="7"/>
+      <c r="P12" s="7"/>
+      <c r="Q12" s="7"/>
+      <c r="R12" s="7"/>
+      <c r="S12" s="7"/>
+      <c r="T12" s="7"/>
+      <c r="U12" s="7"/>
+      <c r="V12" s="7"/>
+      <c r="W12" s="7"/>
+      <c r="X12" s="7"/>
+      <c r="Y12" s="7"/>
+      <c r="Z12" s="7"/>
+      <c r="AA12" s="7"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="K12" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L12" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M12" s="11"/>
-      <c r="N12" s="11"/>
-      <c r="O12" s="11"/>
-      <c r="P12" s="11"/>
-      <c r="Q12" s="11"/>
-      <c r="R12" s="11"/>
-      <c r="S12" s="11"/>
-      <c r="T12" s="11"/>
-      <c r="U12" s="11"/>
-      <c r="V12" s="11"/>
-      <c r="W12" s="11"/>
-      <c r="X12" s="11"/>
-      <c r="Y12" s="11"/>
-      <c r="Z12" s="11"/>
-      <c r="AA12" s="11"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="7" t="s">
+      <c r="B13" s="2" t="s">
         <v>59</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="C13" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C13" s="5" t="s">
-        <v>61</v>
-      </c>
-      <c r="D13" s="9">
+      <c r="D13" s="5">
         <v>3.0</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="5">
         <v>4.0</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="5">
         <v>4.0</v>
       </c>
-      <c r="G13" s="9">
+      <c r="G13" s="5">
         <f t="shared" si="1"/>
         <v>24</v>
       </c>
-      <c r="H13" s="5" t="s">
+      <c r="H13" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="I13" s="6">
+        <v>45573.0</v>
+      </c>
+      <c r="J13" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="I13" s="10">
-        <v>45573.0</v>
-      </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L13" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M13" s="7"/>
+      <c r="N13" s="7"/>
+      <c r="O13" s="7"/>
+      <c r="P13" s="7"/>
+      <c r="Q13" s="7"/>
+      <c r="R13" s="7"/>
+      <c r="S13" s="7"/>
+      <c r="T13" s="7"/>
+      <c r="U13" s="7"/>
+      <c r="V13" s="7"/>
+      <c r="W13" s="7"/>
+      <c r="X13" s="7"/>
+      <c r="Y13" s="7"/>
+      <c r="Z13" s="7"/>
+      <c r="AA13" s="7"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="K13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L13" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M13" s="11"/>
-      <c r="N13" s="11"/>
-      <c r="O13" s="11"/>
-      <c r="P13" s="11"/>
-      <c r="Q13" s="11"/>
-      <c r="R13" s="11"/>
-      <c r="S13" s="11"/>
-      <c r="T13" s="11"/>
-      <c r="U13" s="11"/>
-      <c r="V13" s="11"/>
-      <c r="W13" s="11"/>
-      <c r="X13" s="11"/>
-      <c r="Y13" s="11"/>
-      <c r="Z13" s="11"/>
-      <c r="AA13" s="11"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="7" t="s">
+      <c r="B14" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="C14" s="4" t="s">
         <v>65</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D14" s="9">
+      <c r="D14" s="5">
         <v>2.0</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="5">
         <v>3.0</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="5">
         <v>3.0</v>
       </c>
-      <c r="G14" s="9">
+      <c r="G14" s="5">
         <f t="shared" si="1"/>
         <v>36</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I14" s="6">
+        <v>45568.0</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="I14" s="10">
-        <v>45568.0</v>
-      </c>
-      <c r="J14" s="5" t="s">
+      <c r="K14" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="L14" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="M14" s="7"/>
+      <c r="N14" s="7"/>
+      <c r="O14" s="7"/>
+      <c r="P14" s="7"/>
+      <c r="Q14" s="7"/>
+      <c r="R14" s="7"/>
+      <c r="S14" s="7"/>
+      <c r="T14" s="7"/>
+      <c r="U14" s="7"/>
+      <c r="V14" s="7"/>
+      <c r="W14" s="7"/>
+      <c r="X14" s="7"/>
+      <c r="Y14" s="7"/>
+      <c r="Z14" s="7"/>
+      <c r="AA14" s="7"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B15" s="10" t="s">
         <v>68</v>
       </c>
-      <c r="K14" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L14" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="M14" s="11"/>
-      <c r="N14" s="11"/>
-      <c r="O14" s="11"/>
-      <c r="P14" s="11"/>
-      <c r="Q14" s="11"/>
-      <c r="R14" s="11"/>
-      <c r="S14" s="11"/>
-      <c r="T14" s="11"/>
-      <c r="U14" s="11"/>
-      <c r="V14" s="11"/>
-      <c r="W14" s="11"/>
-      <c r="X14" s="11"/>
-      <c r="Y14" s="11"/>
-      <c r="Z14" s="11"/>
-      <c r="AA14" s="11"/>
-    </row>
-    <row r="15" ht="37.5" customHeight="1">
-      <c r="A15" s="7" t="s">
-        <v>64</v>
-      </c>
-      <c r="B15" s="13" t="s">
+      <c r="C15" s="2" t="s">
         <v>69</v>
       </c>
-      <c r="C15" s="6" t="s">
-        <v>70</v>
-      </c>
-      <c r="D15" s="9">
+      <c r="D15" s="5">
         <v>3.0</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="5">
         <v>2.0</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="5">
         <v>1.0</v>
       </c>
-      <c r="G15" s="9">
+      <c r="G15" s="5">
         <f t="shared" si="1"/>
         <v>12</v>
       </c>
-      <c r="H15" s="5" t="s">
-        <v>67</v>
-      </c>
-      <c r="I15" s="10">
+      <c r="H15" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="I15" s="6">
         <v>45561.0</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="J15" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="K15" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="K15" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="L15" s="7" t="s">
+      <c r="L15" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="M15" s="11"/>
-      <c r="N15" s="11"/>
-      <c r="O15" s="11"/>
-      <c r="P15" s="11"/>
-      <c r="Q15" s="11"/>
-      <c r="R15" s="11"/>
-      <c r="S15" s="11"/>
-      <c r="T15" s="11"/>
-      <c r="U15" s="11"/>
-      <c r="V15" s="11"/>
-      <c r="W15" s="11"/>
-      <c r="X15" s="11"/>
-      <c r="Y15" s="11"/>
-      <c r="Z15" s="11"/>
-      <c r="AA15" s="11"/>
+      <c r="M15" s="7"/>
+      <c r="N15" s="7"/>
+      <c r="O15" s="7"/>
+      <c r="P15" s="7"/>
+      <c r="Q15" s="7"/>
+      <c r="R15" s="7"/>
+      <c r="S15" s="7"/>
+      <c r="T15" s="7"/>
+      <c r="U15" s="7"/>
+      <c r="V15" s="7"/>
+      <c r="W15" s="7"/>
+      <c r="X15" s="7"/>
+      <c r="Y15" s="7"/>
+      <c r="Z15" s="7"/>
+      <c r="AA15" s="7"/>
     </row>
     <row r="16" ht="15.75" customHeight="1">
-      <c r="A16" s="11"/>
-      <c r="B16" s="14"/>
-      <c r="C16" s="11"/>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="15"/>
-      <c r="G16" s="15"/>
-      <c r="H16" s="11"/>
-      <c r="I16" s="16"/>
-      <c r="J16" s="17"/>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11"/>
-      <c r="M16" s="11"/>
-      <c r="N16" s="11"/>
-      <c r="O16" s="11"/>
-      <c r="P16" s="11"/>
-      <c r="Q16" s="11"/>
-      <c r="R16" s="11"/>
-      <c r="S16" s="11"/>
-      <c r="T16" s="11"/>
-      <c r="U16" s="11"/>
-      <c r="V16" s="11"/>
-      <c r="W16" s="11"/>
-      <c r="X16" s="11"/>
-      <c r="Y16" s="11"/>
-      <c r="Z16" s="11"/>
-      <c r="AA16" s="11"/>
+      <c r="A16" s="7"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="7"/>
+      <c r="D16" s="12"/>
+      <c r="E16" s="12"/>
+      <c r="F16" s="12"/>
+      <c r="G16" s="12"/>
+      <c r="H16" s="7"/>
+      <c r="I16" s="13"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="7"/>
+      <c r="L16" s="7"/>
+      <c r="M16" s="7"/>
+      <c r="N16" s="7"/>
+      <c r="O16" s="7"/>
+      <c r="P16" s="7"/>
+      <c r="Q16" s="7"/>
+      <c r="R16" s="7"/>
+      <c r="S16" s="7"/>
+      <c r="T16" s="7"/>
+      <c r="U16" s="7"/>
+      <c r="V16" s="7"/>
+      <c r="W16" s="7"/>
+      <c r="X16" s="7"/>
+      <c r="Y16" s="7"/>
+      <c r="Z16" s="7"/>
+      <c r="AA16" s="7"/>
     </row>
     <row r="17" ht="15.75" customHeight="1">
-      <c r="A17" s="11"/>
-      <c r="B17" s="14"/>
-      <c r="C17" s="11"/>
-      <c r="D17" s="15"/>
-      <c r="E17" s="15"/>
-      <c r="F17" s="15"/>
-      <c r="G17" s="15"/>
-      <c r="H17" s="11"/>
-      <c r="I17" s="16"/>
-      <c r="J17" s="11"/>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11"/>
-      <c r="M17" s="11"/>
-      <c r="N17" s="11"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="11"/>
-      <c r="T17" s="11"/>
-      <c r="U17" s="11"/>
-      <c r="V17" s="11"/>
-      <c r="W17" s="11"/>
-      <c r="X17" s="11"/>
-      <c r="Y17" s="11"/>
-      <c r="Z17" s="11"/>
-      <c r="AA17" s="11"/>
+      <c r="A17" s="7"/>
+      <c r="B17" s="11"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="12"/>
+      <c r="E17" s="12"/>
+      <c r="F17" s="12"/>
+      <c r="G17" s="12"/>
+      <c r="H17" s="7"/>
+      <c r="I17" s="13"/>
+      <c r="J17" s="7"/>
+      <c r="K17" s="7"/>
+      <c r="L17" s="7"/>
+      <c r="M17" s="7"/>
+      <c r="N17" s="7"/>
+      <c r="O17" s="7"/>
+      <c r="P17" s="7"/>
+      <c r="Q17" s="7"/>
+      <c r="R17" s="7"/>
+      <c r="S17" s="7"/>
+      <c r="T17" s="7"/>
+      <c r="U17" s="7"/>
+      <c r="V17" s="7"/>
+      <c r="W17" s="7"/>
+      <c r="X17" s="7"/>
+      <c r="Y17" s="7"/>
+      <c r="Z17" s="7"/>
+      <c r="AA17" s="7"/>
     </row>
     <row r="18" ht="15.75" customHeight="1">
-      <c r="A18" s="11"/>
-      <c r="B18" s="14"/>
-      <c r="C18" s="11"/>
-      <c r="D18" s="15"/>
-      <c r="E18" s="15"/>
-      <c r="F18" s="15"/>
-      <c r="G18" s="15"/>
-      <c r="H18" s="11"/>
-      <c r="I18" s="16"/>
-      <c r="J18" s="17"/>
-      <c r="K18" s="11"/>
-      <c r="L18" s="11"/>
-      <c r="M18" s="11"/>
-      <c r="N18" s="11"/>
-      <c r="O18" s="11"/>
-      <c r="P18" s="11"/>
-      <c r="Q18" s="11"/>
-      <c r="R18" s="11"/>
-      <c r="S18" s="11"/>
-      <c r="T18" s="11"/>
-      <c r="U18" s="11"/>
-      <c r="V18" s="11"/>
-      <c r="W18" s="11"/>
-      <c r="X18" s="11"/>
-      <c r="Y18" s="11"/>
-      <c r="Z18" s="11"/>
-      <c r="AA18" s="11"/>
+      <c r="A18" s="7"/>
+      <c r="B18" s="11"/>
+      <c r="C18" s="7"/>
+      <c r="D18" s="12"/>
+      <c r="E18" s="12"/>
+      <c r="F18" s="12"/>
+      <c r="G18" s="12"/>
+      <c r="H18" s="7"/>
+      <c r="I18" s="13"/>
+      <c r="J18" s="14"/>
+      <c r="K18" s="7"/>
+      <c r="L18" s="7"/>
+      <c r="M18" s="7"/>
+      <c r="N18" s="7"/>
+      <c r="O18" s="7"/>
+      <c r="P18" s="7"/>
+      <c r="Q18" s="7"/>
+      <c r="R18" s="7"/>
+      <c r="S18" s="7"/>
+      <c r="T18" s="7"/>
+      <c r="U18" s="7"/>
+      <c r="V18" s="7"/>
+      <c r="W18" s="7"/>
+      <c r="X18" s="7"/>
+      <c r="Y18" s="7"/>
+      <c r="Z18" s="7"/>
+      <c r="AA18" s="7"/>
     </row>
     <row r="19" ht="15.75" customHeight="1">
-      <c r="A19" s="11"/>
-      <c r="B19" s="14"/>
-      <c r="C19" s="11"/>
-      <c r="D19" s="15"/>
-      <c r="E19" s="15"/>
-      <c r="F19" s="15"/>
-      <c r="G19" s="15"/>
-      <c r="H19" s="11"/>
-      <c r="I19" s="16"/>
-      <c r="J19" s="17"/>
-      <c r="K19" s="11"/>
-      <c r="L19" s="11"/>
-      <c r="M19" s="11"/>
-      <c r="N19" s="11"/>
-      <c r="O19" s="11"/>
-      <c r="P19" s="11"/>
-      <c r="Q19" s="11"/>
-      <c r="R19" s="11"/>
-      <c r="S19" s="11"/>
-      <c r="T19" s="11"/>
-      <c r="U19" s="11"/>
-      <c r="V19" s="11"/>
-      <c r="W19" s="11"/>
-      <c r="X19" s="11"/>
-      <c r="Y19" s="11"/>
-      <c r="Z19" s="11"/>
-      <c r="AA19" s="11"/>
+      <c r="A19" s="7"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="12"/>
+      <c r="E19" s="12"/>
+      <c r="F19" s="12"/>
+      <c r="G19" s="12"/>
+      <c r="H19" s="7"/>
+      <c r="I19" s="13"/>
+      <c r="J19" s="14"/>
+      <c r="K19" s="7"/>
+      <c r="L19" s="7"/>
+      <c r="M19" s="7"/>
+      <c r="N19" s="7"/>
+      <c r="O19" s="7"/>
+      <c r="P19" s="7"/>
+      <c r="Q19" s="7"/>
+      <c r="R19" s="7"/>
+      <c r="S19" s="7"/>
+      <c r="T19" s="7"/>
+      <c r="U19" s="7"/>
+      <c r="V19" s="7"/>
+      <c r="W19" s="7"/>
+      <c r="X19" s="7"/>
+      <c r="Y19" s="7"/>
+      <c r="Z19" s="7"/>
+      <c r="AA19" s="7"/>
     </row>
     <row r="20" ht="15.75" customHeight="1">
-      <c r="A20" s="11"/>
-      <c r="B20" s="14"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="15"/>
-      <c r="E20" s="15"/>
-      <c r="F20" s="15"/>
-      <c r="G20" s="15"/>
-      <c r="H20" s="11"/>
-      <c r="I20" s="16"/>
-      <c r="J20" s="17"/>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11"/>
-      <c r="M20" s="11"/>
-      <c r="N20" s="11"/>
-      <c r="O20" s="11"/>
-      <c r="P20" s="11"/>
-      <c r="Q20" s="11"/>
-      <c r="R20" s="11"/>
-      <c r="S20" s="11"/>
-      <c r="T20" s="11"/>
-      <c r="U20" s="11"/>
-      <c r="V20" s="11"/>
-      <c r="W20" s="11"/>
-      <c r="X20" s="11"/>
-      <c r="Y20" s="11"/>
-      <c r="Z20" s="11"/>
-      <c r="AA20" s="11"/>
+      <c r="A20" s="7"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="7"/>
+      <c r="D20" s="12"/>
+      <c r="E20" s="12"/>
+      <c r="F20" s="12"/>
+      <c r="G20" s="12"/>
+      <c r="H20" s="7"/>
+      <c r="I20" s="13"/>
+      <c r="J20" s="14"/>
+      <c r="K20" s="7"/>
+      <c r="L20" s="7"/>
+      <c r="M20" s="7"/>
+      <c r="N20" s="7"/>
+      <c r="O20" s="7"/>
+      <c r="P20" s="7"/>
+      <c r="Q20" s="7"/>
+      <c r="R20" s="7"/>
+      <c r="S20" s="7"/>
+      <c r="T20" s="7"/>
+      <c r="U20" s="7"/>
+      <c r="V20" s="7"/>
+      <c r="W20" s="7"/>
+      <c r="X20" s="7"/>
+      <c r="Y20" s="7"/>
+      <c r="Z20" s="7"/>
+      <c r="AA20" s="7"/>
     </row>
     <row r="21" ht="15.75" customHeight="1">
-      <c r="A21" s="11"/>
-      <c r="B21" s="14"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="15"/>
-      <c r="E21" s="15"/>
-      <c r="F21" s="15"/>
-      <c r="G21" s="15"/>
-      <c r="H21" s="11"/>
-      <c r="I21" s="16"/>
-      <c r="J21" s="17"/>
-      <c r="K21" s="11"/>
-      <c r="L21" s="11"/>
-      <c r="M21" s="11"/>
-      <c r="N21" s="11"/>
-      <c r="O21" s="11"/>
-      <c r="P21" s="11"/>
-      <c r="Q21" s="11"/>
-      <c r="R21" s="11"/>
-      <c r="S21" s="11"/>
-      <c r="T21" s="11"/>
-      <c r="U21" s="11"/>
-      <c r="V21" s="11"/>
-      <c r="W21" s="11"/>
-      <c r="X21" s="11"/>
-      <c r="Y21" s="11"/>
-      <c r="Z21" s="11"/>
-      <c r="AA21" s="11"/>
+      <c r="A21" s="7"/>
+      <c r="B21" s="11"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="12"/>
+      <c r="E21" s="12"/>
+      <c r="F21" s="12"/>
+      <c r="G21" s="12"/>
+      <c r="H21" s="7"/>
+      <c r="I21" s="13"/>
+      <c r="J21" s="14"/>
+      <c r="K21" s="7"/>
+      <c r="L21" s="7"/>
+      <c r="M21" s="7"/>
+      <c r="N21" s="7"/>
+      <c r="O21" s="7"/>
+      <c r="P21" s="7"/>
+      <c r="Q21" s="7"/>
+      <c r="R21" s="7"/>
+      <c r="S21" s="7"/>
+      <c r="T21" s="7"/>
+      <c r="U21" s="7"/>
+      <c r="V21" s="7"/>
+      <c r="W21" s="7"/>
+      <c r="X21" s="7"/>
+      <c r="Y21" s="7"/>
+      <c r="Z21" s="7"/>
+      <c r="AA21" s="7"/>
     </row>
     <row r="22" ht="15.75" customHeight="1">
-      <c r="A22" s="11"/>
-      <c r="B22" s="14"/>
-      <c r="C22" s="11"/>
-      <c r="D22" s="15"/>
-      <c r="E22" s="15"/>
-      <c r="F22" s="15"/>
-      <c r="G22" s="15"/>
-      <c r="H22" s="11"/>
-      <c r="I22" s="16"/>
-      <c r="J22" s="17"/>
-      <c r="K22" s="11"/>
-      <c r="L22" s="11"/>
-      <c r="M22" s="11"/>
-      <c r="N22" s="11"/>
-      <c r="O22" s="11"/>
-      <c r="P22" s="11"/>
-      <c r="Q22" s="11"/>
-      <c r="R22" s="11"/>
-      <c r="S22" s="11"/>
-      <c r="T22" s="11"/>
-      <c r="U22" s="11"/>
-      <c r="V22" s="11"/>
-      <c r="W22" s="11"/>
-      <c r="X22" s="11"/>
-      <c r="Y22" s="11"/>
-      <c r="Z22" s="11"/>
-      <c r="AA22" s="11"/>
+      <c r="A22" s="7"/>
+      <c r="B22" s="11"/>
+      <c r="C22" s="7"/>
+      <c r="D22" s="12"/>
+      <c r="E22" s="12"/>
+      <c r="F22" s="12"/>
+      <c r="G22" s="12"/>
+      <c r="H22" s="7"/>
+      <c r="I22" s="13"/>
+      <c r="J22" s="14"/>
+      <c r="K22" s="7"/>
+      <c r="L22" s="7"/>
+      <c r="M22" s="7"/>
+      <c r="N22" s="7"/>
+      <c r="O22" s="7"/>
+      <c r="P22" s="7"/>
+      <c r="Q22" s="7"/>
+      <c r="R22" s="7"/>
+      <c r="S22" s="7"/>
+      <c r="T22" s="7"/>
+      <c r="U22" s="7"/>
+      <c r="V22" s="7"/>
+      <c r="W22" s="7"/>
+      <c r="X22" s="7"/>
+      <c r="Y22" s="7"/>
+      <c r="Z22" s="7"/>
+      <c r="AA22" s="7"/>
     </row>
     <row r="23" ht="15.75" customHeight="1">
-      <c r="A23" s="11"/>
-      <c r="B23" s="11"/>
-      <c r="C23" s="11"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="11"/>
-      <c r="I23" s="11"/>
-      <c r="J23" s="11"/>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11"/>
-      <c r="M23" s="11"/>
-      <c r="N23" s="11"/>
-      <c r="O23" s="11"/>
-      <c r="P23" s="11"/>
-      <c r="Q23" s="11"/>
-      <c r="R23" s="11"/>
-      <c r="S23" s="11"/>
-      <c r="T23" s="11"/>
-      <c r="U23" s="11"/>
-      <c r="V23" s="11"/>
-      <c r="W23" s="11"/>
-      <c r="X23" s="11"/>
-      <c r="Y23" s="11"/>
-      <c r="Z23" s="11"/>
-      <c r="AA23" s="11"/>
+      <c r="A23" s="7"/>
+      <c r="B23" s="7"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7"/>
+      <c r="K23" s="7"/>
+      <c r="L23" s="7"/>
+      <c r="M23" s="7"/>
+      <c r="N23" s="7"/>
+      <c r="O23" s="7"/>
+      <c r="P23" s="7"/>
+      <c r="Q23" s="7"/>
+      <c r="R23" s="7"/>
+      <c r="S23" s="7"/>
+      <c r="T23" s="7"/>
+      <c r="U23" s="7"/>
+      <c r="V23" s="7"/>
+      <c r="W23" s="7"/>
+      <c r="X23" s="7"/>
+      <c r="Y23" s="7"/>
+      <c r="Z23" s="7"/>
+      <c r="AA23" s="7"/>
     </row>
     <row r="24" ht="15.75" customHeight="1">
-      <c r="A24" s="7"/>
-      <c r="B24" s="7"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="15"/>
-      <c r="E24" s="15"/>
-      <c r="F24" s="15"/>
-      <c r="G24" s="11"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="11"/>
-      <c r="J24" s="7"/>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11"/>
-      <c r="M24" s="11"/>
-      <c r="N24" s="11"/>
-      <c r="O24" s="11"/>
-      <c r="P24" s="11"/>
-      <c r="Q24" s="11"/>
-      <c r="R24" s="11"/>
-      <c r="S24" s="11"/>
-      <c r="T24" s="11"/>
-      <c r="U24" s="11"/>
-      <c r="V24" s="11"/>
-      <c r="W24" s="11"/>
-      <c r="X24" s="11"/>
-      <c r="Y24" s="11"/>
-      <c r="Z24" s="11"/>
-      <c r="AA24" s="11"/>
+      <c r="A24" s="4"/>
+      <c r="B24" s="4"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="12"/>
+      <c r="E24" s="12"/>
+      <c r="F24" s="12"/>
+      <c r="G24" s="7"/>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="4"/>
+      <c r="K24" s="7"/>
+      <c r="L24" s="7"/>
+      <c r="M24" s="7"/>
+      <c r="N24" s="7"/>
+      <c r="O24" s="7"/>
+      <c r="P24" s="7"/>
+      <c r="Q24" s="7"/>
+      <c r="R24" s="7"/>
+      <c r="S24" s="7"/>
+      <c r="T24" s="7"/>
+      <c r="U24" s="7"/>
+      <c r="V24" s="7"/>
+      <c r="W24" s="7"/>
+      <c r="X24" s="7"/>
+      <c r="Y24" s="7"/>
+      <c r="Z24" s="7"/>
+      <c r="AA24" s="7"/>
     </row>
     <row r="25" ht="15.75" customHeight="1">
-      <c r="A25" s="7"/>
-      <c r="B25" s="7"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="15"/>
-      <c r="E25" s="15"/>
-      <c r="F25" s="15"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="11"/>
-      <c r="I25" s="11"/>
-      <c r="J25" s="7"/>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11"/>
-      <c r="M25" s="11"/>
-      <c r="N25" s="11"/>
-      <c r="O25" s="11"/>
-      <c r="P25" s="11"/>
-      <c r="Q25" s="11"/>
-      <c r="R25" s="11"/>
-      <c r="S25" s="11"/>
-      <c r="T25" s="11"/>
-      <c r="U25" s="11"/>
-      <c r="V25" s="11"/>
-      <c r="W25" s="11"/>
-      <c r="X25" s="11"/>
-      <c r="Y25" s="11"/>
-      <c r="Z25" s="11"/>
-      <c r="AA25" s="11"/>
+      <c r="A25" s="4"/>
+      <c r="B25" s="4"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="12"/>
+      <c r="E25" s="12"/>
+      <c r="F25" s="12"/>
+      <c r="G25" s="7"/>
+      <c r="H25" s="7"/>
+      <c r="I25" s="7"/>
+      <c r="J25" s="4"/>
+      <c r="K25" s="7"/>
+      <c r="L25" s="7"/>
+      <c r="M25" s="7"/>
+      <c r="N25" s="7"/>
+      <c r="O25" s="7"/>
+      <c r="P25" s="7"/>
+      <c r="Q25" s="7"/>
+      <c r="R25" s="7"/>
+      <c r="S25" s="7"/>
+      <c r="T25" s="7"/>
+      <c r="U25" s="7"/>
+      <c r="V25" s="7"/>
+      <c r="W25" s="7"/>
+      <c r="X25" s="7"/>
+      <c r="Y25" s="7"/>
+      <c r="Z25" s="7"/>
+      <c r="AA25" s="7"/>
     </row>
     <row r="26" ht="15.75" customHeight="1">
-      <c r="A26" s="7"/>
-      <c r="B26" s="7"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="15"/>
-      <c r="E26" s="15"/>
-      <c r="F26" s="15"/>
-      <c r="G26" s="11"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="11"/>
-      <c r="J26" s="7"/>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11"/>
-      <c r="M26" s="11"/>
-      <c r="N26" s="11"/>
-      <c r="O26" s="11"/>
-      <c r="P26" s="11"/>
-      <c r="Q26" s="11"/>
-      <c r="R26" s="11"/>
-      <c r="S26" s="11"/>
-      <c r="T26" s="11"/>
-      <c r="U26" s="11"/>
-      <c r="V26" s="11"/>
-      <c r="W26" s="11"/>
-      <c r="X26" s="11"/>
-      <c r="Y26" s="11"/>
-      <c r="Z26" s="11"/>
-      <c r="AA26" s="11"/>
+      <c r="A26" s="4"/>
+      <c r="B26" s="4"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="12"/>
+      <c r="E26" s="12"/>
+      <c r="F26" s="12"/>
+      <c r="G26" s="7"/>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="4"/>
+      <c r="K26" s="7"/>
+      <c r="L26" s="7"/>
+      <c r="M26" s="7"/>
+      <c r="N26" s="7"/>
+      <c r="O26" s="7"/>
+      <c r="P26" s="7"/>
+      <c r="Q26" s="7"/>
+      <c r="R26" s="7"/>
+      <c r="S26" s="7"/>
+      <c r="T26" s="7"/>
+      <c r="U26" s="7"/>
+      <c r="V26" s="7"/>
+      <c r="W26" s="7"/>
+      <c r="X26" s="7"/>
+      <c r="Y26" s="7"/>
+      <c r="Z26" s="7"/>
+      <c r="AA26" s="7"/>
     </row>
     <row r="27" ht="15.75" customHeight="1">
-      <c r="A27" s="7"/>
-      <c r="B27" s="7"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="15"/>
-      <c r="E27" s="15"/>
-      <c r="F27" s="15"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="11"/>
-      <c r="I27" s="11"/>
-      <c r="J27" s="7"/>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11"/>
-      <c r="M27" s="11"/>
-      <c r="N27" s="11"/>
-      <c r="O27" s="11"/>
-      <c r="P27" s="11"/>
-      <c r="Q27" s="11"/>
-      <c r="R27" s="11"/>
-      <c r="S27" s="11"/>
-      <c r="T27" s="11"/>
-      <c r="U27" s="11"/>
-      <c r="V27" s="11"/>
-      <c r="W27" s="11"/>
-      <c r="X27" s="11"/>
-      <c r="Y27" s="11"/>
-      <c r="Z27" s="11"/>
-      <c r="AA27" s="11"/>
+      <c r="A27" s="4"/>
+      <c r="B27" s="4"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="12"/>
+      <c r="E27" s="12"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="7"/>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="4"/>
+      <c r="K27" s="7"/>
+      <c r="L27" s="7"/>
+      <c r="M27" s="7"/>
+      <c r="N27" s="7"/>
+      <c r="O27" s="7"/>
+      <c r="P27" s="7"/>
+      <c r="Q27" s="7"/>
+      <c r="R27" s="7"/>
+      <c r="S27" s="7"/>
+      <c r="T27" s="7"/>
+      <c r="U27" s="7"/>
+      <c r="V27" s="7"/>
+      <c r="W27" s="7"/>
+      <c r="X27" s="7"/>
+      <c r="Y27" s="7"/>
+      <c r="Z27" s="7"/>
+      <c r="AA27" s="7"/>
     </row>
     <row r="28" ht="15.75" customHeight="1">
-      <c r="A28" s="7"/>
-      <c r="D28" s="15"/>
-      <c r="E28" s="15"/>
-      <c r="F28" s="15"/>
-      <c r="G28" s="11"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="11"/>
-      <c r="J28" s="7"/>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11"/>
-      <c r="M28" s="11"/>
-      <c r="N28" s="11"/>
-      <c r="O28" s="11"/>
-      <c r="P28" s="11"/>
-      <c r="Q28" s="11"/>
-      <c r="R28" s="11"/>
-      <c r="S28" s="11"/>
-      <c r="T28" s="11"/>
-      <c r="U28" s="11"/>
-      <c r="V28" s="11"/>
-      <c r="W28" s="11"/>
-      <c r="X28" s="11"/>
-      <c r="Y28" s="11"/>
-      <c r="Z28" s="11"/>
-      <c r="AA28" s="11"/>
+      <c r="A28" s="4"/>
+      <c r="D28" s="12"/>
+      <c r="E28" s="12"/>
+      <c r="F28" s="12"/>
+      <c r="G28" s="7"/>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="4"/>
+      <c r="K28" s="7"/>
+      <c r="L28" s="7"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="7"/>
+      <c r="P28" s="7"/>
+      <c r="Q28" s="7"/>
+      <c r="R28" s="7"/>
+      <c r="S28" s="7"/>
+      <c r="T28" s="7"/>
+      <c r="U28" s="7"/>
+      <c r="V28" s="7"/>
+      <c r="W28" s="7"/>
+      <c r="X28" s="7"/>
+      <c r="Y28" s="7"/>
+      <c r="Z28" s="7"/>
+      <c r="AA28" s="7"/>
     </row>
     <row r="29" ht="15.75" customHeight="1">
-      <c r="A29" s="7"/>
-      <c r="B29" s="7"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="15"/>
-      <c r="E29" s="15"/>
-      <c r="F29" s="15"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="11"/>
-      <c r="J29" s="7"/>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11"/>
-      <c r="M29" s="11"/>
-      <c r="N29" s="11"/>
-      <c r="O29" s="11"/>
-      <c r="P29" s="11"/>
-      <c r="Q29" s="11"/>
-      <c r="R29" s="11"/>
-      <c r="S29" s="11"/>
-      <c r="T29" s="11"/>
-      <c r="U29" s="11"/>
-      <c r="V29" s="11"/>
-      <c r="W29" s="11"/>
-      <c r="X29" s="11"/>
-      <c r="Y29" s="11"/>
-      <c r="Z29" s="11"/>
-      <c r="AA29" s="11"/>
+      <c r="A29" s="4"/>
+      <c r="B29" s="4"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="12"/>
+      <c r="E29" s="12"/>
+      <c r="F29" s="12"/>
+      <c r="G29" s="7"/>
+      <c r="H29" s="7"/>
+      <c r="I29" s="7"/>
+      <c r="J29" s="4"/>
+      <c r="K29" s="7"/>
+      <c r="L29" s="7"/>
+      <c r="M29" s="7"/>
+      <c r="N29" s="7"/>
+      <c r="O29" s="7"/>
+      <c r="P29" s="7"/>
+      <c r="Q29" s="7"/>
+      <c r="R29" s="7"/>
+      <c r="S29" s="7"/>
+      <c r="T29" s="7"/>
+      <c r="U29" s="7"/>
+      <c r="V29" s="7"/>
+      <c r="W29" s="7"/>
+      <c r="X29" s="7"/>
+      <c r="Y29" s="7"/>
+      <c r="Z29" s="7"/>
+      <c r="AA29" s="7"/>
     </row>
     <row r="30" ht="15.75" customHeight="1">
-      <c r="A30" s="7"/>
-      <c r="B30" s="7"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="15"/>
-      <c r="E30" s="11"/>
-      <c r="F30" s="11"/>
-      <c r="G30" s="11"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="11"/>
-      <c r="J30" s="7"/>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11"/>
-      <c r="M30" s="11"/>
-      <c r="N30" s="11"/>
-      <c r="O30" s="11"/>
-      <c r="P30" s="11"/>
-      <c r="Q30" s="11"/>
-      <c r="R30" s="11"/>
-      <c r="S30" s="11"/>
-      <c r="T30" s="11"/>
-      <c r="U30" s="11"/>
-      <c r="V30" s="11"/>
-      <c r="W30" s="11"/>
-      <c r="X30" s="11"/>
-      <c r="Y30" s="11"/>
-      <c r="Z30" s="11"/>
-      <c r="AA30" s="11"/>
+      <c r="A30" s="4"/>
+      <c r="B30" s="4"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="12"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="7"/>
+      <c r="G30" s="7"/>
+      <c r="H30" s="7"/>
+      <c r="I30" s="7"/>
+      <c r="J30" s="4"/>
+      <c r="K30" s="7"/>
+      <c r="L30" s="7"/>
+      <c r="M30" s="7"/>
+      <c r="N30" s="7"/>
+      <c r="O30" s="7"/>
+      <c r="P30" s="7"/>
+      <c r="Q30" s="7"/>
+      <c r="R30" s="7"/>
+      <c r="S30" s="7"/>
+      <c r="T30" s="7"/>
+      <c r="U30" s="7"/>
+      <c r="V30" s="7"/>
+      <c r="W30" s="7"/>
+      <c r="X30" s="7"/>
+      <c r="Y30" s="7"/>
+      <c r="Z30" s="7"/>
+      <c r="AA30" s="7"/>
     </row>
     <row r="31" ht="15.75" customHeight="1">
-      <c r="A31" s="11"/>
-      <c r="B31" s="11"/>
-      <c r="C31" s="11"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="11"/>
-      <c r="J31" s="11"/>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11"/>
-      <c r="M31" s="11"/>
-      <c r="N31" s="11"/>
-      <c r="O31" s="11"/>
-      <c r="P31" s="11"/>
-      <c r="Q31" s="11"/>
-      <c r="R31" s="11"/>
-      <c r="S31" s="11"/>
-      <c r="T31" s="11"/>
-      <c r="U31" s="11"/>
-      <c r="V31" s="11"/>
-      <c r="W31" s="11"/>
-      <c r="X31" s="11"/>
-      <c r="Y31" s="11"/>
-      <c r="Z31" s="11"/>
-      <c r="AA31" s="11"/>
+      <c r="A31" s="7"/>
+      <c r="B31" s="7"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="7"/>
+      <c r="E31" s="7"/>
+      <c r="F31" s="7"/>
+      <c r="G31" s="7"/>
+      <c r="H31" s="7"/>
+      <c r="I31" s="7"/>
+      <c r="J31" s="7"/>
+      <c r="K31" s="7"/>
+      <c r="L31" s="7"/>
+      <c r="M31" s="7"/>
+      <c r="N31" s="7"/>
+      <c r="O31" s="7"/>
+      <c r="P31" s="7"/>
+      <c r="Q31" s="7"/>
+      <c r="R31" s="7"/>
+      <c r="S31" s="7"/>
+      <c r="T31" s="7"/>
+      <c r="U31" s="7"/>
+      <c r="V31" s="7"/>
+      <c r="W31" s="7"/>
+      <c r="X31" s="7"/>
+      <c r="Y31" s="7"/>
+      <c r="Z31" s="7"/>
+      <c r="AA31" s="7"/>
     </row>
     <row r="32" ht="15.75" customHeight="1"/>
     <row r="33" ht="15.75" customHeight="1">
-      <c r="A33" s="11"/>
-      <c r="B33" s="11"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="15"/>
-      <c r="E33" s="15"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="15"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="11"/>
-      <c r="J33" s="17"/>
-      <c r="K33" s="11"/>
-      <c r="L33" s="11"/>
-      <c r="M33" s="11"/>
-      <c r="N33" s="11"/>
-      <c r="O33" s="11"/>
-      <c r="P33" s="11"/>
-      <c r="Q33" s="11"/>
-      <c r="R33" s="11"/>
-      <c r="S33" s="11"/>
-      <c r="T33" s="11"/>
-      <c r="U33" s="11"/>
-      <c r="V33" s="11"/>
-      <c r="W33" s="11"/>
-      <c r="X33" s="11"/>
-      <c r="Y33" s="11"/>
-      <c r="Z33" s="11"/>
-      <c r="AA33" s="11"/>
+      <c r="A33" s="7"/>
+      <c r="B33" s="7"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="12"/>
+      <c r="E33" s="12"/>
+      <c r="F33" s="7"/>
+      <c r="G33" s="12"/>
+      <c r="H33" s="7"/>
+      <c r="I33" s="7"/>
+      <c r="J33" s="14"/>
+      <c r="K33" s="7"/>
+      <c r="L33" s="7"/>
+      <c r="M33" s="7"/>
+      <c r="N33" s="7"/>
+      <c r="O33" s="7"/>
+      <c r="P33" s="7"/>
+      <c r="Q33" s="7"/>
+      <c r="R33" s="7"/>
+      <c r="S33" s="7"/>
+      <c r="T33" s="7"/>
+      <c r="U33" s="7"/>
+      <c r="V33" s="7"/>
+      <c r="W33" s="7"/>
+      <c r="X33" s="7"/>
+      <c r="Y33" s="7"/>
+      <c r="Z33" s="7"/>
+      <c r="AA33" s="7"/>
     </row>
     <row r="34" ht="15.75" customHeight="1">
-      <c r="A34" s="11"/>
-      <c r="B34" s="11"/>
-      <c r="C34" s="7"/>
-      <c r="D34" s="15"/>
-      <c r="E34" s="15"/>
-      <c r="F34" s="11"/>
-      <c r="G34" s="15"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="11"/>
-      <c r="J34" s="17"/>
-      <c r="K34" s="11"/>
-      <c r="L34" s="11"/>
-      <c r="M34" s="11"/>
-      <c r="N34" s="11"/>
-      <c r="O34" s="11"/>
-      <c r="P34" s="11"/>
-      <c r="Q34" s="11"/>
-      <c r="R34" s="11"/>
-      <c r="S34" s="11"/>
-      <c r="T34" s="11"/>
-      <c r="U34" s="11"/>
-      <c r="V34" s="11"/>
-      <c r="W34" s="11"/>
-      <c r="X34" s="11"/>
-      <c r="Y34" s="11"/>
-      <c r="Z34" s="11"/>
-      <c r="AA34" s="11"/>
+      <c r="A34" s="7"/>
+      <c r="B34" s="7"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="12"/>
+      <c r="E34" s="12"/>
+      <c r="F34" s="7"/>
+      <c r="G34" s="12"/>
+      <c r="H34" s="7"/>
+      <c r="I34" s="7"/>
+      <c r="J34" s="14"/>
+      <c r="K34" s="7"/>
+      <c r="L34" s="7"/>
+      <c r="M34" s="7"/>
+      <c r="N34" s="7"/>
+      <c r="O34" s="7"/>
+      <c r="P34" s="7"/>
+      <c r="Q34" s="7"/>
+      <c r="R34" s="7"/>
+      <c r="S34" s="7"/>
+      <c r="T34" s="7"/>
+      <c r="U34" s="7"/>
+      <c r="V34" s="7"/>
+      <c r="W34" s="7"/>
+      <c r="X34" s="7"/>
+      <c r="Y34" s="7"/>
+      <c r="Z34" s="7"/>
+      <c r="AA34" s="7"/>
     </row>
     <row r="35" ht="15.75" customHeight="1">
-      <c r="A35" s="11"/>
-      <c r="B35" s="11"/>
-      <c r="C35" s="7"/>
-      <c r="D35" s="15"/>
-      <c r="E35" s="15"/>
-      <c r="F35" s="11"/>
-      <c r="G35" s="15"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="11"/>
-      <c r="J35" s="11"/>
-      <c r="K35" s="11"/>
-      <c r="L35" s="11"/>
-      <c r="M35" s="11"/>
-      <c r="N35" s="11"/>
-      <c r="O35" s="11"/>
-      <c r="P35" s="11"/>
-      <c r="Q35" s="11"/>
-      <c r="R35" s="11"/>
-      <c r="S35" s="11"/>
-      <c r="T35" s="11"/>
-      <c r="U35" s="11"/>
-      <c r="V35" s="11"/>
-      <c r="W35" s="11"/>
-      <c r="X35" s="11"/>
-      <c r="Y35" s="11"/>
-      <c r="Z35" s="11"/>
-      <c r="AA35" s="11"/>
+      <c r="A35" s="7"/>
+      <c r="B35" s="7"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="12"/>
+      <c r="E35" s="12"/>
+      <c r="F35" s="7"/>
+      <c r="G35" s="12"/>
+      <c r="H35" s="7"/>
+      <c r="I35" s="7"/>
+      <c r="J35" s="7"/>
+      <c r="K35" s="7"/>
+      <c r="L35" s="7"/>
+      <c r="M35" s="7"/>
+      <c r="N35" s="7"/>
+      <c r="O35" s="7"/>
+      <c r="P35" s="7"/>
+      <c r="Q35" s="7"/>
+      <c r="R35" s="7"/>
+      <c r="S35" s="7"/>
+      <c r="T35" s="7"/>
+      <c r="U35" s="7"/>
+      <c r="V35" s="7"/>
+      <c r="W35" s="7"/>
+      <c r="X35" s="7"/>
+      <c r="Y35" s="7"/>
+      <c r="Z35" s="7"/>
+      <c r="AA35" s="7"/>
     </row>
     <row r="36" ht="15.75" customHeight="1">
-      <c r="A36" s="11"/>
-      <c r="B36" s="11"/>
-      <c r="C36" s="7"/>
-      <c r="D36" s="15"/>
-      <c r="E36" s="15"/>
-      <c r="F36" s="11"/>
-      <c r="G36" s="15"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="11"/>
-      <c r="J36" s="11"/>
-      <c r="K36" s="11"/>
-      <c r="L36" s="11"/>
-      <c r="M36" s="11"/>
-      <c r="N36" s="11"/>
-      <c r="O36" s="11"/>
-      <c r="P36" s="11"/>
-      <c r="Q36" s="11"/>
-      <c r="R36" s="11"/>
-      <c r="S36" s="11"/>
-      <c r="T36" s="11"/>
-      <c r="U36" s="11"/>
-      <c r="V36" s="11"/>
-      <c r="W36" s="11"/>
-      <c r="X36" s="11"/>
-      <c r="Y36" s="11"/>
-      <c r="Z36" s="11"/>
-      <c r="AA36" s="11"/>
+      <c r="A36" s="7"/>
+      <c r="B36" s="7"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="12"/>
+      <c r="E36" s="12"/>
+      <c r="F36" s="7"/>
+      <c r="G36" s="12"/>
+      <c r="H36" s="7"/>
+      <c r="I36" s="7"/>
+      <c r="J36" s="7"/>
+      <c r="K36" s="7"/>
+      <c r="L36" s="7"/>
+      <c r="M36" s="7"/>
+      <c r="N36" s="7"/>
+      <c r="O36" s="7"/>
+      <c r="P36" s="7"/>
+      <c r="Q36" s="7"/>
+      <c r="R36" s="7"/>
+      <c r="S36" s="7"/>
+      <c r="T36" s="7"/>
+      <c r="U36" s="7"/>
+      <c r="V36" s="7"/>
+      <c r="W36" s="7"/>
+      <c r="X36" s="7"/>
+      <c r="Y36" s="7"/>
+      <c r="Z36" s="7"/>
+      <c r="AA36" s="7"/>
     </row>
     <row r="37" ht="15.75" customHeight="1"/>
     <row r="38" ht="15.75" customHeight="1"/>

</xml_diff>